<commit_message>
Repaired enums in fluid names and parameters. First to do: fluid factory
</commit_message>
<xml_diff>
--- a/lista_nazw.xlsx
+++ b/lista_nazw.xlsx
@@ -1146,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B73482-1FE5-492E-95CC-325361080563}">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1160,7 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,8 +1178,12 @@
         <f>_xlfn.CONCAT(UPPER(D1),"(Arrays.asList(""",D1,""")),")</f>
         <v>1-BUTENE(Arrays.asList("1-Butene")),</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O1" t="str">
+        <f>_xlfn.CONCAT(UPPER(D1),"(""",D1,"""),")</f>
+        <v>1-BUTENE("1-Butene"),</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1197,8 +1201,12 @@
         <f t="shared" ref="J2:J65" si="1">_xlfn.CONCAT(UPPER(D2),"(Arrays.asList(""",D2,""")),")</f>
         <v>ACETONE(Arrays.asList("Acetone")),</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O65" si="2">_xlfn.CONCAT(UPPER(D2),"(""",D2,"""),")</f>
+        <v>ACETONE("Acetone"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1216,8 +1224,12 @@
         <f t="shared" si="1"/>
         <v>AIR(Arrays.asList("Air")),</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O3" t="str">
+        <f t="shared" si="2"/>
+        <v>AIR("Air"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1235,8 +1247,12 @@
         <f t="shared" si="1"/>
         <v>AMMONIA(Arrays.asList("Ammonia")),</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v>AMMONIA("Ammonia"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1254,8 +1270,12 @@
         <f t="shared" si="1"/>
         <v>ARGON(Arrays.asList("Argon")),</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>ARGON("Argon"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1273,8 +1293,12 @@
         <f t="shared" si="1"/>
         <v>BENZENE(Arrays.asList("Benzene")),</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>BENZENE("Benzene"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1292,8 +1316,12 @@
         <f t="shared" si="1"/>
         <v>CARBONDIOXIDE(Arrays.asList("CarbonDioxide")),</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>CARBONDIOXIDE("CarbonDioxide"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1311,8 +1339,12 @@
         <f t="shared" si="1"/>
         <v>CARBONMONOXIDE(Arrays.asList("CarbonMonoxide")),</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>CARBONMONOXIDE("CarbonMonoxide"),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1330,8 +1362,12 @@
         <f t="shared" si="1"/>
         <v>CARBONYLSULFIDE(Arrays.asList("CarbonylSulfide")),</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>CARBONYLSULFIDE("CarbonylSulfide"),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1349,8 +1385,12 @@
         <f t="shared" si="1"/>
         <v>CYCLOHEXANE(Arrays.asList("CycloHexane")),</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v>CYCLOHEXANE("CycloHexane"),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1368,8 +1408,12 @@
         <f t="shared" si="1"/>
         <v>CYCLOPROPANE(Arrays.asList("CycloPropane")),</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O11" t="str">
+        <f t="shared" si="2"/>
+        <v>CYCLOPROPANE("CycloPropane"),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1387,8 +1431,12 @@
         <f t="shared" si="1"/>
         <v>CYCLOPENTANE(Arrays.asList("Cyclopentane")),</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v>CYCLOPENTANE("Cyclopentane"),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1406,8 +1454,12 @@
         <f t="shared" si="1"/>
         <v>D4(Arrays.asList("D4")),</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>D4("D4"),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1425,8 +1477,12 @@
         <f t="shared" si="1"/>
         <v>D5(Arrays.asList("D5")),</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>D5("D5"),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1444,8 +1500,12 @@
         <f t="shared" si="1"/>
         <v>D6(Arrays.asList("D6")),</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>D6("D6"),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1463,8 +1523,12 @@
         <f t="shared" si="1"/>
         <v>DEUTERIUM(Arrays.asList("Deuterium")),</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O16" t="str">
+        <f t="shared" si="2"/>
+        <v>DEUTERIUM("Deuterium"),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1482,8 +1546,12 @@
         <f t="shared" si="1"/>
         <v>DICHLOROETHANE(Arrays.asList("Dichloroethane")),</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O17" t="str">
+        <f t="shared" si="2"/>
+        <v>DICHLOROETHANE("Dichloroethane"),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1501,8 +1569,12 @@
         <f t="shared" si="1"/>
         <v>DIETHYLETHER(Arrays.asList("DiethylEther")),</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="O18" t="str">
+        <f t="shared" si="2"/>
+        <v>DIETHYLETHER("DiethylEther"),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1520,8 +1592,12 @@
         <f t="shared" si="1"/>
         <v>DIMETHYLCARBONATE(Arrays.asList("DimethylCarbonate")),</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O19" t="str">
+        <f t="shared" si="2"/>
+        <v>DIMETHYLCARBONATE("DimethylCarbonate"),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1539,8 +1615,12 @@
         <f t="shared" si="1"/>
         <v>DIMETHYLETHER(Arrays.asList("DimethylEther")),</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O20" t="str">
+        <f t="shared" si="2"/>
+        <v>DIMETHYLETHER("DimethylEther"),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1558,8 +1638,12 @@
         <f t="shared" si="1"/>
         <v>ETHANE(Arrays.asList("Ethane")),</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O21" t="str">
+        <f t="shared" si="2"/>
+        <v>ETHANE("Ethane"),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1577,8 +1661,12 @@
         <f t="shared" si="1"/>
         <v>ETHANOL(Arrays.asList("Ethanol")),</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O22" t="str">
+        <f t="shared" si="2"/>
+        <v>ETHANOL("Ethanol"),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1596,8 +1684,12 @@
         <f t="shared" si="1"/>
         <v>ETHYLBENZENE(Arrays.asList("EthylBenzene")),</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O23" t="str">
+        <f t="shared" si="2"/>
+        <v>ETHYLBENZENE("EthylBenzene"),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1615,8 +1707,12 @@
         <f t="shared" si="1"/>
         <v>ETHYLENE(Arrays.asList("Ethylene")),</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O24" t="str">
+        <f t="shared" si="2"/>
+        <v>ETHYLENE("Ethylene"),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1634,8 +1730,12 @@
         <f t="shared" si="1"/>
         <v>ETHYLENEOXIDE(Arrays.asList("EthyleneOxide")),</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O25" t="str">
+        <f t="shared" si="2"/>
+        <v>ETHYLENEOXIDE("EthyleneOxide"),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1653,8 +1753,12 @@
         <f t="shared" si="1"/>
         <v>FLUORINE(Arrays.asList("Fluorine")),</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O26" t="str">
+        <f t="shared" si="2"/>
+        <v>FLUORINE("Fluorine"),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1672,8 +1776,12 @@
         <f t="shared" si="1"/>
         <v>HFE143M(Arrays.asList("HFE143m")),</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O27" t="str">
+        <f t="shared" si="2"/>
+        <v>HFE143M("HFE143m"),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1691,8 +1799,12 @@
         <f t="shared" si="1"/>
         <v>HEAVYWATER(Arrays.asList("HeavyWater")),</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O28" t="str">
+        <f t="shared" si="2"/>
+        <v>HEAVYWATER("HeavyWater"),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1710,8 +1822,12 @@
         <f t="shared" si="1"/>
         <v>HELIUM(Arrays.asList("Helium")),</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O29" t="str">
+        <f t="shared" si="2"/>
+        <v>HELIUM("Helium"),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1729,8 +1845,12 @@
         <f t="shared" si="1"/>
         <v>HYDROGEN(Arrays.asList("Hydrogen")),</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="O30" t="str">
+        <f t="shared" si="2"/>
+        <v>HYDROGEN("Hydrogen"),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1748,8 +1868,12 @@
         <f t="shared" si="1"/>
         <v>HYDROGENCHLORIDE(Arrays.asList("HydrogenChloride")),</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O31" t="str">
+        <f t="shared" si="2"/>
+        <v>HYDROGENCHLORIDE("HydrogenChloride"),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1767,8 +1891,12 @@
         <f t="shared" si="1"/>
         <v>HYDROGENSULFIDE(Arrays.asList("HydrogenSulfide")),</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O32" t="str">
+        <f t="shared" si="2"/>
+        <v>HYDROGENSULFIDE("HydrogenSulfide"),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1786,8 +1914,12 @@
         <f t="shared" si="1"/>
         <v>ISOBUTANE(Arrays.asList("IsoButane")),</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O33" t="str">
+        <f t="shared" si="2"/>
+        <v>ISOBUTANE("IsoButane"),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1805,8 +1937,12 @@
         <f t="shared" si="1"/>
         <v>ISOBUTENE(Arrays.asList("IsoButene")),</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O34" t="str">
+        <f t="shared" si="2"/>
+        <v>ISOBUTENE("IsoButene"),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1824,8 +1960,12 @@
         <f t="shared" si="1"/>
         <v>ISOHEXANE(Arrays.asList("Isohexane")),</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O35" t="str">
+        <f t="shared" si="2"/>
+        <v>ISOHEXANE("Isohexane"),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1843,8 +1983,12 @@
         <f t="shared" si="1"/>
         <v>ISOPENTANE(Arrays.asList("Isopentane")),</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O36" t="str">
+        <f t="shared" si="2"/>
+        <v>ISOPENTANE("Isopentane"),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1862,8 +2006,12 @@
         <f t="shared" si="1"/>
         <v>KRYPTON(Arrays.asList("Krypton")),</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O37" t="str">
+        <f t="shared" si="2"/>
+        <v>KRYPTON("Krypton"),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1881,8 +2029,12 @@
         <f t="shared" si="1"/>
         <v>MD2M(Arrays.asList("MD2M")),</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O38" t="str">
+        <f t="shared" si="2"/>
+        <v>MD2M("MD2M"),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1900,8 +2052,12 @@
         <f t="shared" si="1"/>
         <v>MD3M(Arrays.asList("MD3M")),</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O39" t="str">
+        <f t="shared" si="2"/>
+        <v>MD3M("MD3M"),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1919,8 +2075,12 @@
         <f t="shared" si="1"/>
         <v>MD4M(Arrays.asList("MD4M")),</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O40" t="str">
+        <f t="shared" si="2"/>
+        <v>MD4M("MD4M"),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1938,8 +2098,12 @@
         <f t="shared" si="1"/>
         <v>MDM(Arrays.asList("MDM")),</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O41" t="str">
+        <f t="shared" si="2"/>
+        <v>MDM("MDM"),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1957,8 +2121,12 @@
         <f t="shared" si="1"/>
         <v>MM(Arrays.asList("MM")),</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O42" t="str">
+        <f t="shared" si="2"/>
+        <v>MM("MM"),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1976,8 +2144,12 @@
         <f t="shared" si="1"/>
         <v>METHANE(Arrays.asList("Methane")),</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O43" t="str">
+        <f t="shared" si="2"/>
+        <v>METHANE("Methane"),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1995,8 +2167,12 @@
         <f t="shared" si="1"/>
         <v>METHANOL(Arrays.asList("Methanol")),</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O44" t="str">
+        <f t="shared" si="2"/>
+        <v>METHANOL("Methanol"),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -2014,8 +2190,12 @@
         <f t="shared" si="1"/>
         <v>METHYLLINOLEATE(Arrays.asList("MethylLinoleate")),</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O45" t="str">
+        <f t="shared" si="2"/>
+        <v>METHYLLINOLEATE("MethylLinoleate"),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2033,8 +2213,12 @@
         <f t="shared" si="1"/>
         <v>METHYLLINOLENATE(Arrays.asList("MethylLinolenate")),</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O46" t="str">
+        <f t="shared" si="2"/>
+        <v>METHYLLINOLENATE("MethylLinolenate"),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -2052,8 +2236,12 @@
         <f t="shared" si="1"/>
         <v>METHYLOLEATE(Arrays.asList("MethylOleate")),</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O47" t="str">
+        <f t="shared" si="2"/>
+        <v>METHYLOLEATE("MethylOleate"),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -2071,8 +2259,12 @@
         <f t="shared" si="1"/>
         <v>METHYLPALMITATE(Arrays.asList("MethylPalmitate")),</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O48" t="str">
+        <f t="shared" si="2"/>
+        <v>METHYLPALMITATE("MethylPalmitate"),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -2090,8 +2282,12 @@
         <f t="shared" si="1"/>
         <v>METHYLSTEARATE(Arrays.asList("MethylStearate")),</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O49" t="str">
+        <f t="shared" si="2"/>
+        <v>METHYLSTEARATE("MethylStearate"),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -2109,8 +2305,12 @@
         <f t="shared" si="1"/>
         <v>NEON(Arrays.asList("Neon")),</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O50" t="str">
+        <f t="shared" si="2"/>
+        <v>NEON("Neon"),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -2128,8 +2328,12 @@
         <f t="shared" si="1"/>
         <v>NEOPENTANE(Arrays.asList("Neopentane")),</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O51" t="str">
+        <f t="shared" si="2"/>
+        <v>NEOPENTANE("Neopentane"),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -2147,8 +2351,12 @@
         <f t="shared" si="1"/>
         <v>NITROGEN(Arrays.asList("Nitrogen")),</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O52" t="str">
+        <f t="shared" si="2"/>
+        <v>NITROGEN("Nitrogen"),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -2166,8 +2374,12 @@
         <f t="shared" si="1"/>
         <v>NITROUSOXIDE(Arrays.asList("NitrousOxide")),</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O53" t="str">
+        <f t="shared" si="2"/>
+        <v>NITROUSOXIDE("NitrousOxide"),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -2185,8 +2397,12 @@
         <f t="shared" si="1"/>
         <v>NOVEC649(Arrays.asList("Novec649")),</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O54" t="str">
+        <f t="shared" si="2"/>
+        <v>NOVEC649("Novec649"),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -2204,8 +2420,12 @@
         <f t="shared" si="1"/>
         <v>ORTHODEUTERIUM(Arrays.asList("OrthoDeuterium")),</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O55" t="str">
+        <f t="shared" si="2"/>
+        <v>ORTHODEUTERIUM("OrthoDeuterium"),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -2223,8 +2443,12 @@
         <f t="shared" si="1"/>
         <v>ORTHOHYDROGEN(Arrays.asList("OrthoHydrogen")),</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O56" t="str">
+        <f t="shared" si="2"/>
+        <v>ORTHOHYDROGEN("OrthoHydrogen"),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -2242,8 +2466,12 @@
         <f t="shared" si="1"/>
         <v>OXYGEN(Arrays.asList("Oxygen")),</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O57" t="str">
+        <f t="shared" si="2"/>
+        <v>OXYGEN("Oxygen"),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -2261,8 +2489,12 @@
         <f t="shared" si="1"/>
         <v>PARADEUTERIUM(Arrays.asList("ParaDeuterium")),</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O58" t="str">
+        <f t="shared" si="2"/>
+        <v>PARADEUTERIUM("ParaDeuterium"),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -2280,8 +2512,12 @@
         <f t="shared" si="1"/>
         <v>PARAHYDROGEN(Arrays.asList("ParaHydrogen")),</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O59" t="str">
+        <f t="shared" si="2"/>
+        <v>PARAHYDROGEN("ParaHydrogen"),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -2299,8 +2535,12 @@
         <f t="shared" si="1"/>
         <v>PROPYLENE(Arrays.asList("Propylene")),</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O60" t="str">
+        <f t="shared" si="2"/>
+        <v>PROPYLENE("Propylene"),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -2318,8 +2558,12 @@
         <f t="shared" si="1"/>
         <v>PROPYNE(Arrays.asList("Propyne")),</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O61" t="str">
+        <f t="shared" si="2"/>
+        <v>PROPYNE("Propyne"),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -2337,8 +2581,12 @@
         <f t="shared" si="1"/>
         <v>R11(Arrays.asList("R11")),</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O62" t="str">
+        <f t="shared" si="2"/>
+        <v>R11("R11"),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -2356,8 +2604,12 @@
         <f t="shared" si="1"/>
         <v>R113(Arrays.asList("R113")),</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O63" t="str">
+        <f t="shared" si="2"/>
+        <v>R113("R113"),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -2375,8 +2627,12 @@
         <f t="shared" si="1"/>
         <v>R114(Arrays.asList("R114")),</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O64" t="str">
+        <f t="shared" si="2"/>
+        <v>R114("R114"),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -2394,8 +2650,12 @@
         <f t="shared" si="1"/>
         <v>R115(Arrays.asList("R115")),</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O65" t="str">
+        <f t="shared" si="2"/>
+        <v>R115("R115"),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -2403,18 +2663,22 @@
         <v>65</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F122" si="2">UPPER( _xlfn.CONCAT(D66,",") )</f>
+        <f t="shared" ref="F66:F122" si="3">UPPER( _xlfn.CONCAT(D66,",") )</f>
         <v>R116,</v>
       </c>
       <c r="I66" t="s">
         <v>187</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J122" si="3">_xlfn.CONCAT(UPPER(D66),"(Arrays.asList(""",D66,""")),")</f>
+        <f t="shared" ref="J66:J122" si="4">_xlfn.CONCAT(UPPER(D66),"(Arrays.asList(""",D66,""")),")</f>
         <v>R116(Arrays.asList("R116")),</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O66" t="str">
+        <f t="shared" ref="O66:O122" si="5">_xlfn.CONCAT(UPPER(D66),"(""",D66,"""),")</f>
+        <v>R116("R116"),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -2422,18 +2686,22 @@
         <v>66</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R12,</v>
       </c>
       <c r="I67" t="s">
         <v>188</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R12(Arrays.asList("R12")),</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O67" t="str">
+        <f t="shared" si="5"/>
+        <v>R12("R12"),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -2441,18 +2709,22 @@
         <v>67</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R123,</v>
       </c>
       <c r="I68" t="s">
         <v>189</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R123(Arrays.asList("R123")),</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O68" t="str">
+        <f t="shared" si="5"/>
+        <v>R123("R123"),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -2460,18 +2732,22 @@
         <v>68</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R1233ZD(E),</v>
       </c>
       <c r="I69" t="s">
         <v>190</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R1233ZD(E)(Arrays.asList("R1233zd(E)")),</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O69" t="str">
+        <f t="shared" si="5"/>
+        <v>R1233ZD(E)("R1233zd(E)"),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -2479,18 +2755,22 @@
         <v>69</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R1234YF,</v>
       </c>
       <c r="I70" t="s">
         <v>191</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R1234YF(Arrays.asList("R1234yf")),</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O70" t="str">
+        <f t="shared" si="5"/>
+        <v>R1234YF("R1234yf"),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -2498,18 +2778,22 @@
         <v>70</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R1234ZE(E),</v>
       </c>
       <c r="I71" t="s">
         <v>192</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R1234ZE(E)(Arrays.asList("R1234ze(E)")),</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O71" t="str">
+        <f t="shared" si="5"/>
+        <v>R1234ZE(E)("R1234ze(E)"),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -2517,18 +2801,22 @@
         <v>71</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R1234ZE(Z),</v>
       </c>
       <c r="I72" t="s">
         <v>193</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R1234ZE(Z)(Arrays.asList("R1234ze(Z)")),</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O72" t="str">
+        <f t="shared" si="5"/>
+        <v>R1234ZE(Z)("R1234ze(Z)"),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -2536,18 +2824,22 @@
         <v>72</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R124,</v>
       </c>
       <c r="I73" t="s">
         <v>194</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R124(Arrays.asList("R124")),</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O73" t="str">
+        <f t="shared" si="5"/>
+        <v>R124("R124"),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -2555,18 +2847,22 @@
         <v>73</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R125,</v>
       </c>
       <c r="I74" t="s">
         <v>195</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R125(Arrays.asList("R125")),</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O74" t="str">
+        <f t="shared" si="5"/>
+        <v>R125("R125"),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -2574,18 +2870,22 @@
         <v>74</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R13,</v>
       </c>
       <c r="I75" t="s">
         <v>196</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R13(Arrays.asList("R13")),</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O75" t="str">
+        <f t="shared" si="5"/>
+        <v>R13("R13"),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -2593,18 +2893,22 @@
         <v>75</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R134A,</v>
       </c>
       <c r="I76" t="s">
         <v>197</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R134A(Arrays.asList("R134a")),</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O76" t="str">
+        <f t="shared" si="5"/>
+        <v>R134A("R134a"),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2612,18 +2916,22 @@
         <v>76</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R13I1,</v>
       </c>
       <c r="I77" t="s">
         <v>198</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R13I1(Arrays.asList("R13I1")),</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O77" t="str">
+        <f t="shared" si="5"/>
+        <v>R13I1("R13I1"),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -2631,18 +2939,22 @@
         <v>77</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R14,</v>
       </c>
       <c r="I78" t="s">
         <v>199</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R14(Arrays.asList("R14")),</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O78" t="str">
+        <f t="shared" si="5"/>
+        <v>R14("R14"),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -2650,18 +2962,22 @@
         <v>78</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R141B,</v>
       </c>
       <c r="I79" t="s">
         <v>200</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R141B(Arrays.asList("R141b")),</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O79" t="str">
+        <f t="shared" si="5"/>
+        <v>R141B("R141b"),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -2669,18 +2985,22 @@
         <v>79</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R142B,</v>
       </c>
       <c r="I80" t="s">
         <v>201</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R142B(Arrays.asList("R142b")),</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O80" t="str">
+        <f t="shared" si="5"/>
+        <v>R142B("R142b"),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -2688,18 +3008,22 @@
         <v>80</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R143A,</v>
       </c>
       <c r="I81" t="s">
         <v>202</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R143A(Arrays.asList("R143a")),</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O81" t="str">
+        <f t="shared" si="5"/>
+        <v>R143A("R143a"),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -2707,18 +3031,22 @@
         <v>81</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R152A,</v>
       </c>
       <c r="I82" t="s">
         <v>203</v>
       </c>
       <c r="J82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R152A(Arrays.asList("R152A")),</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O82" t="str">
+        <f t="shared" si="5"/>
+        <v>R152A("R152A"),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -2726,18 +3054,22 @@
         <v>82</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R161,</v>
       </c>
       <c r="I83" t="s">
         <v>204</v>
       </c>
       <c r="J83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R161(Arrays.asList("R161")),</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O83" t="str">
+        <f t="shared" si="5"/>
+        <v>R161("R161"),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -2745,18 +3077,22 @@
         <v>83</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R21,</v>
       </c>
       <c r="I84" t="s">
         <v>205</v>
       </c>
       <c r="J84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R21(Arrays.asList("R21")),</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O84" t="str">
+        <f t="shared" si="5"/>
+        <v>R21("R21"),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -2764,18 +3100,22 @@
         <v>84</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R218,</v>
       </c>
       <c r="I85" t="s">
         <v>206</v>
       </c>
       <c r="J85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R218(Arrays.asList("R218")),</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O85" t="str">
+        <f t="shared" si="5"/>
+        <v>R218("R218"),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -2783,18 +3123,22 @@
         <v>85</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R22,</v>
       </c>
       <c r="I86" t="s">
         <v>207</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R22(Arrays.asList("R22")),</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O86" t="str">
+        <f t="shared" si="5"/>
+        <v>R22("R22"),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -2802,18 +3146,22 @@
         <v>86</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R227EA,</v>
       </c>
       <c r="I87" t="s">
         <v>208</v>
       </c>
       <c r="J87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R227EA(Arrays.asList("R227EA")),</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O87" t="str">
+        <f t="shared" si="5"/>
+        <v>R227EA("R227EA"),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -2821,18 +3169,22 @@
         <v>87</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R23,</v>
       </c>
       <c r="I88" t="s">
         <v>209</v>
       </c>
       <c r="J88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R23(Arrays.asList("R23")),</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O88" t="str">
+        <f t="shared" si="5"/>
+        <v>R23("R23"),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -2840,18 +3192,22 @@
         <v>88</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R236EA,</v>
       </c>
       <c r="I89" t="s">
         <v>210</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R236EA(Arrays.asList("R236EA")),</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O89" t="str">
+        <f t="shared" si="5"/>
+        <v>R236EA("R236EA"),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -2859,18 +3215,22 @@
         <v>89</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R236FA,</v>
       </c>
       <c r="I90" t="s">
         <v>211</v>
       </c>
       <c r="J90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R236FA(Arrays.asList("R236FA")),</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O90" t="str">
+        <f t="shared" si="5"/>
+        <v>R236FA("R236FA"),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -2878,18 +3238,22 @@
         <v>90</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R245CA,</v>
       </c>
       <c r="I91" t="s">
         <v>212</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R245CA(Arrays.asList("R245ca")),</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O91" t="str">
+        <f t="shared" si="5"/>
+        <v>R245CA("R245ca"),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -2897,18 +3261,22 @@
         <v>91</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R245FA,</v>
       </c>
       <c r="I92" t="s">
         <v>213</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R245FA(Arrays.asList("R245fa")),</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O92" t="str">
+        <f t="shared" si="5"/>
+        <v>R245FA("R245fa"),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2916,18 +3284,22 @@
         <v>92</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R32,</v>
       </c>
       <c r="I93" t="s">
         <v>214</v>
       </c>
       <c r="J93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R32(Arrays.asList("R32")),</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O93" t="str">
+        <f t="shared" si="5"/>
+        <v>R32("R32"),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -2935,18 +3307,22 @@
         <v>93</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R365MFC,</v>
       </c>
       <c r="I94" t="s">
         <v>215</v>
       </c>
       <c r="J94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R365MFC(Arrays.asList("R365MFC")),</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O94" t="str">
+        <f t="shared" si="5"/>
+        <v>R365MFC("R365MFC"),</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -2954,18 +3330,22 @@
         <v>94</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R40,</v>
       </c>
       <c r="I95" t="s">
         <v>216</v>
       </c>
       <c r="J95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R40(Arrays.asList("R40")),</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O95" t="str">
+        <f t="shared" si="5"/>
+        <v>R40("R40"),</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -2973,18 +3353,22 @@
         <v>95</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R404A,</v>
       </c>
       <c r="I96" t="s">
         <v>217</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R404A(Arrays.asList("R404A")),</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O96" t="str">
+        <f t="shared" si="5"/>
+        <v>R404A("R404A"),</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -2992,18 +3376,22 @@
         <v>96</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R407C,</v>
       </c>
       <c r="I97" t="s">
         <v>218</v>
       </c>
       <c r="J97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R407C(Arrays.asList("R407C")),</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O97" t="str">
+        <f t="shared" si="5"/>
+        <v>R407C("R407C"),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -3011,18 +3399,22 @@
         <v>97</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R41,</v>
       </c>
       <c r="I98" t="s">
         <v>219</v>
       </c>
       <c r="J98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R41(Arrays.asList("R41")),</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O98" t="str">
+        <f t="shared" si="5"/>
+        <v>R41("R41"),</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -3030,18 +3422,22 @@
         <v>98</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R410A,</v>
       </c>
       <c r="I99" t="s">
         <v>220</v>
       </c>
       <c r="J99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R410A(Arrays.asList("R410A")),</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O99" t="str">
+        <f t="shared" si="5"/>
+        <v>R410A("R410A"),</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -3049,18 +3445,22 @@
         <v>99</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>R507A,</v>
       </c>
       <c r="I100" t="s">
         <v>221</v>
       </c>
       <c r="J100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R507A(Arrays.asList("R507A")),</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O100" t="str">
+        <f t="shared" si="5"/>
+        <v>R507A("R507A"),</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -3068,18 +3468,22 @@
         <v>100</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>RC318,</v>
       </c>
       <c r="I101" t="s">
         <v>222</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>RC318(Arrays.asList("RC318")),</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O101" t="str">
+        <f t="shared" si="5"/>
+        <v>RC318("RC318"),</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
@@ -3087,18 +3491,22 @@
         <v>101</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SES36,</v>
       </c>
       <c r="I102" t="s">
         <v>223</v>
       </c>
       <c r="J102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SES36(Arrays.asList("SES36")),</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O102" t="str">
+        <f t="shared" si="5"/>
+        <v>SES36("SES36"),</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -3106,18 +3514,22 @@
         <v>102</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SULFURDIOXIDE,</v>
       </c>
       <c r="I103" t="s">
         <v>224</v>
       </c>
       <c r="J103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SULFURDIOXIDE(Arrays.asList("SulfurDioxide")),</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="O103" t="str">
+        <f t="shared" si="5"/>
+        <v>SULFURDIOXIDE("SulfurDioxide"),</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
@@ -3125,18 +3537,22 @@
         <v>103</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SULFURHEXAFLUORIDE,</v>
       </c>
       <c r="I104" t="s">
         <v>225</v>
       </c>
       <c r="J104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SULFURHEXAFLUORIDE(Arrays.asList("SulfurHexafluoride")),</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O104" t="str">
+        <f t="shared" si="5"/>
+        <v>SULFURHEXAFLUORIDE("SulfurHexafluoride"),</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -3144,18 +3560,22 @@
         <v>104</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TOLUENE,</v>
       </c>
       <c r="I105" t="s">
         <v>226</v>
       </c>
       <c r="J105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TOLUENE(Arrays.asList("Toluene")),</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O105" t="str">
+        <f t="shared" si="5"/>
+        <v>TOLUENE("Toluene"),</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
@@ -3163,18 +3583,22 @@
         <v>105</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>WATER,</v>
       </c>
       <c r="I106" t="s">
         <v>227</v>
       </c>
       <c r="J106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WATER(Arrays.asList("Water")),</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O106" t="str">
+        <f t="shared" si="5"/>
+        <v>WATER("Water"),</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -3182,18 +3606,22 @@
         <v>106</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>XENON,</v>
       </c>
       <c r="I107" t="s">
         <v>123</v>
       </c>
       <c r="J107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>XENON(Arrays.asList("Xenon")),</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O107" t="str">
+        <f t="shared" si="5"/>
+        <v>XENON("Xenon"),</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -3201,18 +3629,22 @@
         <v>107</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>CIS-2-BUTENE,</v>
       </c>
       <c r="I108" t="s">
         <v>228</v>
       </c>
       <c r="J108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CIS-2-BUTENE(Arrays.asList("cis-2-Butene")),</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O108" t="str">
+        <f t="shared" si="5"/>
+        <v>CIS-2-BUTENE("cis-2-Butene"),</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -3220,18 +3652,22 @@
         <v>108</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>M-XYLENE,</v>
       </c>
       <c r="I109" t="s">
         <v>229</v>
       </c>
       <c r="J109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>M-XYLENE(Arrays.asList("m-Xylene")),</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O109" t="str">
+        <f t="shared" si="5"/>
+        <v>M-XYLENE("m-Xylene"),</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
@@ -3239,18 +3675,22 @@
         <v>109</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-BUTANE,</v>
       </c>
       <c r="I110" t="s">
         <v>230</v>
       </c>
       <c r="J110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-BUTANE(Arrays.asList("n-Butane")),</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O110" t="str">
+        <f t="shared" si="5"/>
+        <v>N-BUTANE("n-Butane"),</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
@@ -3258,18 +3698,22 @@
         <v>110</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-DECANE,</v>
       </c>
       <c r="I111" t="s">
         <v>231</v>
       </c>
       <c r="J111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-DECANE(Arrays.asList("n-Decane")),</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="O111" t="str">
+        <f t="shared" si="5"/>
+        <v>N-DECANE("n-Decane"),</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -3277,18 +3721,22 @@
         <v>111</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-DODECANE,</v>
       </c>
       <c r="I112" t="s">
         <v>232</v>
       </c>
       <c r="J112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-DODECANE(Arrays.asList("n-Dodecane")),</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O112" t="str">
+        <f t="shared" si="5"/>
+        <v>N-DODECANE("n-Dodecane"),</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -3296,18 +3744,22 @@
         <v>112</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-HEPTANE,</v>
       </c>
       <c r="I113" t="s">
         <v>233</v>
       </c>
       <c r="J113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-HEPTANE(Arrays.asList("n-Heptane")),</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O113" t="str">
+        <f t="shared" si="5"/>
+        <v>N-HEPTANE("n-Heptane"),</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -3315,18 +3767,22 @@
         <v>113</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-HEXANE,</v>
       </c>
       <c r="I114" t="s">
         <v>234</v>
       </c>
       <c r="J114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-HEXANE(Arrays.asList("n-Hexane")),</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O114" t="str">
+        <f t="shared" si="5"/>
+        <v>N-HEXANE("n-Hexane"),</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -3334,18 +3790,22 @@
         <v>114</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-NONANE,</v>
       </c>
       <c r="I115" t="s">
         <v>235</v>
       </c>
       <c r="J115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-NONANE(Arrays.asList("n-Nonane")),</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O115" t="str">
+        <f t="shared" si="5"/>
+        <v>N-NONANE("n-Nonane"),</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -3353,18 +3813,22 @@
         <v>115</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-OCTANE,</v>
       </c>
       <c r="I116" t="s">
         <v>236</v>
       </c>
       <c r="J116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-OCTANE(Arrays.asList("n-Octane")),</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O116" t="str">
+        <f t="shared" si="5"/>
+        <v>N-OCTANE("n-Octane"),</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -3372,18 +3836,22 @@
         <v>116</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-PENTANE,</v>
       </c>
       <c r="I117" t="s">
         <v>237</v>
       </c>
       <c r="J117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-PENTANE(Arrays.asList("n-Pentane")),</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O117" t="str">
+        <f t="shared" si="5"/>
+        <v>N-PENTANE("n-Pentane"),</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -3391,18 +3859,22 @@
         <v>117</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-PROPANE,</v>
       </c>
       <c r="I118" t="s">
         <v>238</v>
       </c>
       <c r="J118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-PROPANE(Arrays.asList("n-Propane")),</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="O118" t="str">
+        <f t="shared" si="5"/>
+        <v>N-PROPANE("n-Propane"),</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -3410,18 +3882,22 @@
         <v>118</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N-UNDECANE,</v>
       </c>
       <c r="I119" t="s">
         <v>239</v>
       </c>
       <c r="J119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N-UNDECANE(Arrays.asList("n-Undecane")),</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O119" t="str">
+        <f t="shared" si="5"/>
+        <v>N-UNDECANE("n-Undecane"),</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -3429,18 +3905,22 @@
         <v>119</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>O-XYLENE,</v>
       </c>
       <c r="I120" t="s">
         <v>240</v>
       </c>
       <c r="J120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>O-XYLENE(Arrays.asList("o-Xylene")),</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O120" t="str">
+        <f t="shared" si="5"/>
+        <v>O-XYLENE("o-Xylene"),</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -3448,18 +3928,22 @@
         <v>120</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>P-XYLENE,</v>
       </c>
       <c r="I121" t="s">
         <v>241</v>
       </c>
       <c r="J121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P-XYLENE(Arrays.asList("p-Xylene")),</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="O121" t="str">
+        <f t="shared" si="5"/>
+        <v>P-XYLENE("p-Xylene"),</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -3467,18 +3951,22 @@
         <v>121</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TRANS-2-BUTENE,</v>
       </c>
       <c r="I122" t="s">
         <v>242</v>
       </c>
       <c r="J122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TRANS-2-BUTENE(Arrays.asList("trans-2-Butene")),</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O122" t="str">
+        <f t="shared" si="5"/>
+        <v>TRANS-2-BUTENE("trans-2-Butene"),</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I123" t="s">
         <v>243</v>
       </c>

</xml_diff>